<commit_message>
Update Rollerball System Test Cases.xlsx
</commit_message>
<xml_diff>
--- a/Final_Project 04/Rollerball System Test Cases.xlsx
+++ b/Final_Project 04/Rollerball System Test Cases.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11109"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timothy.stroup\Documents\SequenceDiagrams\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunny/Documents/GitHub/cs414-f18-001-stringCheese/Final_Project 04/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F435B51-BDA2-B443-A960-7AE18D434344}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15510" windowHeight="3500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27640" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -42,31 +43,16 @@
     <t>Register an account</t>
   </si>
   <si>
-    <t>1: Connect to the system
-2: Enter new email an password
-3: Click register</t>
-  </si>
-  <si>
     <t>User account is created</t>
   </si>
   <si>
     <t>Log in to the system</t>
   </si>
   <si>
-    <t>1: Connect to the system
-2: Enter existing email and password
-3: Cick log in</t>
-  </si>
-  <si>
     <t>User is logged in</t>
   </si>
   <si>
     <t>View User Profile</t>
-  </si>
-  <si>
-    <t>1: Connect to the system
-2: Log in
-3: Select View user Profile from menu</t>
   </si>
   <si>
     <t>User Profile is displayed</t>
@@ -98,13 +84,6 @@
   </si>
   <si>
     <t>Send Invitation</t>
-  </si>
-  <si>
-    <t>1: Connect to the system
-2: Log in 
-3: Select Send Invitation/Create Game button
-4: Select Users fom the drop down menu
-5: Click send Invitation</t>
   </si>
   <si>
     <t>Emails are sent to each of the users selected and a single game is created</t>
@@ -174,12 +153,53 @@
   <si>
     <t>Account is deactiavted and user can no longer log in</t>
   </si>
+  <si>
+    <t>1: Connect to the system
+2: Enter new name(meetsavaliya2), email(meet2@ymail.com), and password(meet123)                       
+3: Click register</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1: Connect to the system
+2: Enter existing email(meetsavaliya2) and password(meet123)
+3: Cick log in</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1: Connect to the system
+2: Log in 
+3: Select Send Invitation/Create Game button
+4: Select Users fom the drop down menu
+5: Click send Invitation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1: Connect to the system
+2: Log in
+3: Select View user Profile from menu</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Done</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pass</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rework</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -188,6 +208,23 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Wawati TC"/>
+      <family val="3"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -210,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -218,9 +255,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -497,26 +540,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="131" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.453125" style="2"/>
-    <col min="2" max="2" width="26.7265625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="36" style="2" customWidth="1"/>
-    <col min="4" max="4" width="41.81640625" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="14.453125" style="2"/>
+    <col min="1" max="1" width="14.5" style="2"/>
+    <col min="2" max="2" width="26.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="55" style="2" customWidth="1"/>
+    <col min="4" max="4" width="41.83203125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="14.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -536,161 +579,228 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="56" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="E2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="42" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="E3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="42" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="62.5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="70" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="50" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="56" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="E6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="70" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="62.5" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="70" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="87.5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="94" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="62.5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="56" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="62.5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="70" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="50" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="56" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>